<commit_message>
✨ feat: change layout at entry data , upload photo at data entry based on sKode, Semester, Year
</commit_message>
<xml_diff>
--- a/public/template/FormatEntry.xlsx
+++ b/public/template/FormatEntry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11580"/>
+    <workbookView windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Kode</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Rusak</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Tahun</t>
   </si>
   <si>
     <t>Deskripsi</t>
@@ -961,16 +967,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>18415</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -979,8 +985,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7974330" y="190500"/>
-          <a:ext cx="3954780" cy="1190625"/>
+          <a:off x="7132320" y="190500"/>
+          <a:ext cx="3954780" cy="2028190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1011,9 +1017,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
@@ -1067,6 +1071,32 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Rusak	Satuan dari barang	1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Semester	Semester </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>dari penginputan</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	Ganjil</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Tahun	Tahun dari penginputan	2024</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1289,23 +1319,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="17.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="15.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="9" max="9" width="17.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="17.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:5">
+    <row r="1" customHeight="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1321,6 +1351,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>